<commit_message>
Updated last results from SM
</commit_message>
<xml_diff>
--- a/SM_Inspecion_102924.xlsx
+++ b/SM_Inspecion_102924.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/vanessa_garayburu-caruso_pnnl_gov/Documents/Documents/GitHub/SSS_metabolism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{C6873D16-C439-46AD-890B-AF88953F048E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4743C1DA-7FC1-45FE-89B1-1F82DCE16874}"/>
+  <xr:revisionPtr revIDLastSave="517" documentId="8_{C6873D16-C439-46AD-890B-AF88953F048E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20BFCFE8-5FF7-4008-B26C-9B59F3F666F9}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="12525" xr2:uid="{D067E5FF-B7BE-4CCB-A546-E1FF0B3DFFED}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="12525" activeTab="1" xr2:uid="{D067E5FF-B7BE-4CCB-A546-E1FF0B3DFFED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="11-17-24" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'11-17-24'!$A$1:$J$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$49</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="146">
   <si>
     <t>Site</t>
   </si>
@@ -571,27 +573,15 @@
     <t>Rerun KSD 0.2</t>
   </si>
   <si>
-    <t>KS 0.1 and look at a picture of the stream</t>
-  </si>
-  <si>
     <t>Check metadata to see if this was deployed at a different location after sampling day</t>
   </si>
   <si>
-    <t>KSD 0.1</t>
-  </si>
-  <si>
-    <t>Bad site but KSD 0.1</t>
-  </si>
-  <si>
     <t>Can stay as is or KSD 0.05</t>
   </si>
   <si>
     <t>Lost site always fails, probably doesn't meet metabolism assumption</t>
   </si>
   <si>
-    <t>KS D 0.1</t>
-  </si>
-  <si>
     <t>Remove days with biofouling August 5,6,and 7. Rerun KSD  0.05</t>
   </si>
   <si>
@@ -602,6 +592,54 @@
   </si>
   <si>
     <t>Remove days where depth was changing a lot because of the dam.  Need to remove the whole pulse</t>
+  </si>
+  <si>
+    <t>KS 0.1 and look at a picture of the stream. Tryin 0.08 first</t>
+  </si>
+  <si>
+    <t>KSD 0.1. Trying 0.08 first</t>
+  </si>
+  <si>
+    <t>Bad site but KSD 0.1  Trying 0.08 first</t>
+  </si>
+  <si>
+    <t>KS D 0.1.  Trying 0.08 first</t>
+  </si>
+  <si>
+    <t>Overall very low ER. Mostly positive ER but might need to re-run at 0.08</t>
+  </si>
+  <si>
+    <t>Never goes under saturation</t>
+  </si>
+  <si>
+    <t>Bad site does not meet SM assumptions</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/21 n_eff error not super great still but seems the best </t>
+  </si>
+  <si>
+    <t>11/21 Error ranges for ER a little high</t>
+  </si>
+  <si>
+    <t>11/21 One day with larger error bar for ER but probably not a big deal for the avgs</t>
+  </si>
+  <si>
+    <t>11/21 Model fits are not great and also n_eff are not super ideal. ER is very low check with Bob</t>
+  </si>
+  <si>
+    <t>11/21 Model fits are not great (some blips on the low do) and also n_eff are not super ideal. ER is very low check with Bob</t>
+  </si>
+  <si>
+    <t>11/21 Remove 2 more days at the end? Might not make a big impact</t>
+  </si>
+  <si>
+    <t>11/21 Could remove one more day in the middle. Computation looks good at KSD 0.02</t>
+  </si>
+  <si>
+    <t>11/21 Reruning 0.1 something seems off on the model fits on the tail for some reason. Huge error ranges</t>
   </si>
 </sst>
 </file>
@@ -640,7 +678,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,6 +688,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -752,11 +808,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1266,14 +1440,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E102E9-0757-4782-BA5A-E8CFEF1F8992}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.20703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" style="6" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.41796875" style="4" customWidth="1"/>
@@ -1283,7 +1457,7 @@
     <col min="8" max="8" width="10" style="2" customWidth="1"/>
     <col min="9" max="9" width="14" style="2" customWidth="1"/>
     <col min="10" max="10" width="42.68359375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9.9453125" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="47.68359375" customWidth="1"/>
     <col min="13" max="13" width="16.15625" customWidth="1"/>
   </cols>
@@ -1394,7 +1568,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1440,7 +1614,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1718,7 +1892,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>112</v>
@@ -1744,7 +1918,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1828,7 +2002,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>10</v>
@@ -1856,7 +2030,7 @@
         <v>98</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1903,7 +2077,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1921,7 +2095,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1941,7 +2115,7 @@
         <v>10</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1963,7 +2137,7 @@
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>10</v>
@@ -2018,7 +2192,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -2040,7 +2214,7 @@
         <v>10</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2122,7 +2296,7 @@
       </c>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:11" ht="23.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" ht="23.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5" t="s">
         <v>55</v>
       </c>
@@ -2150,7 +2324,7 @@
         <v>10</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>113</v>
@@ -2169,7 +2343,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="16" t="s">
         <v>57</v>
       </c>
@@ -2222,7 +2396,7 @@
         <v>10</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>104</v>
@@ -2269,7 +2443,7 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>10</v>
@@ -2313,7 +2487,7 @@
         <v>10</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -2384,7 +2558,7 @@
         <v>10</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
@@ -2448,34 +2622,34 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K49" xr:uid="{99E102E9-0757-4782-BA5A-E8CFEF1F8992}"/>
+  <autoFilter ref="A1:M49" xr:uid="{99E102E9-0757-4782-BA5A-E8CFEF1F8992}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576 K12 K7:K8 K10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"Bob"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2483,4 +2657,941 @@
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8CBE01-4BB7-437F-A298-F6FB9342FA88}">
+  <dimension ref="A1:J49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="8.83984375" style="6"/>
+    <col min="2" max="2" width="16.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83984375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="18.578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.41796875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.41796875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.68359375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="33.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="20"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="15"/>
+    </row>
+    <row r="48" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J49" xr:uid="{0D8CBE01-4BB7-437F-A298-F6FB9342FA88}"/>
+  <conditionalFormatting sqref="H1:H49">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:C33 B36:C49">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I49">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Bob"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:E14 E15 C15 D16:E36 D38:E49 E37 C37">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:C35">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Uploaded final files part 2
</commit_message>
<xml_diff>
--- a/SM_Inspecion_102924.xlsx
+++ b/SM_Inspecion_102924.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/vanessa_garayburu-caruso_pnnl_gov/Documents/Documents/GitHub/SSS_metabolism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="522" documentId="8_{C6873D16-C439-46AD-890B-AF88953F048E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FA98EE4-7F31-40DA-B5D9-E436C483BA36}"/>
+  <xr:revisionPtr revIDLastSave="527" documentId="8_{C6873D16-C439-46AD-890B-AF88953F048E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{867CCA30-2455-46A1-9707-2EA58DC8CE3D}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="21840" windowHeight="12525" activeTab="1" xr2:uid="{D067E5FF-B7BE-4CCB-A546-E1FF0B3DFFED}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="13182" firstSheet="1" activeTab="1" xr2:uid="{D067E5FF-B7BE-4CCB-A546-E1FF0B3DFFED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="148">
   <si>
     <t>Site</t>
   </si>
@@ -643,6 +643,9 @@
   </si>
   <si>
     <t>Postive ER</t>
+  </si>
+  <si>
+    <t>OLD ONE MUCH BETTER</t>
   </si>
 </sst>
 </file>
@@ -2656,11 +2659,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8CBE01-4BB7-437F-A298-F6FB9342FA88}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2709,7 +2713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -2814,7 +2818,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -2864,7 +2868,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -2882,7 +2886,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -2965,7 +2969,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
@@ -3065,14 +3069,16 @@
       <c r="I22" s="1"/>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="D23" s="3" t="s">
         <v>10</v>
       </c>
@@ -3083,7 +3089,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
@@ -3169,7 +3175,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5" t="s">
         <v>46</v>
       </c>
@@ -3262,14 +3268,16 @@
       <c r="I33" s="1"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="D34" s="8" t="s">
         <v>10</v>
       </c>
@@ -3282,7 +3290,7 @@
       </c>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" ht="72" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5" t="s">
         <v>54</v>
       </c>
@@ -3355,7 +3363,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="5" t="s">
         <v>58</v>
       </c>
@@ -3389,7 +3397,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="5" t="s">
         <v>61</v>
       </c>
@@ -3423,7 +3431,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="5" t="s">
         <v>63</v>
       </c>
@@ -3459,7 +3467,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="5" t="s">
         <v>65</v>
       </c>
@@ -3477,7 +3485,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5" t="s">
         <v>67</v>
       </c>
@@ -3546,7 +3554,13 @@
       <c r="J49" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J49" xr:uid="{0D8CBE01-4BB7-437F-A298-F6FB9342FA88}"/>
+  <autoFilter ref="A1:J49" xr:uid="{0D8CBE01-4BB7-437F-A298-F6FB9342FA88}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="X"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="H1:H49">
     <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"?"</formula>

</xml_diff>